<commit_message>
Ran ExpediaTestNGRunner file. Test Cases pass as well as the assertions
</commit_message>
<xml_diff>
--- a/com.expedia/src/test/resources/test_data.xlsx
+++ b/com.expedia/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.expedia\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E82C12-11AC-4AED-A5CF-BB9D94CD0939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420D5292-4380-4612-9405-89E322E80D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
@@ -331,9 +331,6 @@
     <t>Mexico</t>
   </si>
   <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>Istanbul</t>
   </si>
   <si>
@@ -368,6 +365,9 @@
   </si>
   <si>
     <t>France</t>
+  </si>
+  <si>
+    <t>South Africa</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1234,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1259,67 +1259,67 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushing expedia test cases. Keep running further tests to deal with 'Access Denied' message
</commit_message>
<xml_diff>
--- a/com.expedia/src/test/resources/test_data.xlsx
+++ b/com.expedia/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.expedia\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622848E3-3D64-448F-BEDD-E7DC9D465D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBCEEE1-9882-4402-AEA7-514F0B186055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
     <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
@@ -361,9 +361,6 @@
     <t>Portugal</t>
   </si>
   <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
     <t>France</t>
   </si>
   <si>
@@ -374,6 +371,9 @@
   </si>
   <si>
     <t>X3</t>
+  </si>
+  <si>
+    <t>Morocco</t>
   </si>
 </sst>
 </file>
@@ -417,11 +417,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1214,7 +1215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DBDB2A-BA3E-4DD2-85D1-84D270436187}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1232,12 +1233,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1249,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F428AD-AE09-447E-9CC1-5B40C17299F3}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1259,7 +1260,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1275,7 +1276,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -1330,15 +1331,16 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding some more Expedia TestCases
</commit_message>
<xml_diff>
--- a/com.expedia/src/test/resources/test_data.xlsx
+++ b/com.expedia/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malik/IdeaProjects/Team1SeleniumBootcamp/com.expedia/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7650CF13-C5CC-544E-A8F5-C36E98F33100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974895CA-4E59-A645-B8F9-AB35217280FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{D923710D-3166-6945-8322-D716FA8B43D1}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <t>Current Alerts</t>
   </si>
   <si>
-    <t>Welcome to Expedia.co.in.</t>
+    <t>Trips</t>
   </si>
 </sst>
 </file>

</xml_diff>